<commit_message>
Definições das consultas e otimizações
Co-authored-by: Pietro Zuntini <pietrozuntini@gmail.com>
</commit_message>
<xml_diff>
--- a/Fase 03 - SBD (Consultas SQL e Otimização)/Tempos.xlsx
+++ b/Fase 03 - SBD (Consultas SQL e Otimização)/Tempos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\educa_brasil\Fase 03 - SBD (Consultas SQL e Otimização)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976631CC-7CBB-4C1E-85FC-C078B42FB027}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC00FC7-4AB1-48FF-A3DB-51CF45557193}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{60C1C061-DBD4-48AD-A7F9-20614BF445A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{60C1C061-DBD4-48AD-A7F9-20614BF445A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,23 +31,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Testes</t>
   </si>
   <si>
-    <t>Tempo</t>
-  </si>
-  <si>
-    <t>Execução sem otimização</t>
+    <t>Consulta 1</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>ÍNDICE</t>
+  </si>
+  <si>
+    <t>LIKE</t>
+  </si>
+  <si>
+    <t>Tempo (ms)</t>
+  </si>
+  <si>
+    <t>Consulta Inicial (JOIN)</t>
+  </si>
+  <si>
+    <t>Consulta 2</t>
+  </si>
+  <si>
+    <t>Diferença com Original (%)</t>
+  </si>
+  <si>
+    <t>Diferença com Anterior (%)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,12 +103,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,45 +454,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0204754B-D6F4-4E2C-9215-C6E014B7E421}">
-  <dimension ref="B2:G5"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="4" width="16.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>30246</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C6" s="2">
+        <v>19094</v>
+      </c>
+      <c r="D6" s="2">
+        <v>36.869999999999997</v>
+      </c>
+      <c r="E6" s="2">
+        <v>36.869999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>16504</v>
+      </c>
+      <c r="D7" s="2">
+        <v>13.56</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45.43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2008</v>
+      </c>
+      <c r="D8" s="2">
+        <v>87.83</v>
+      </c>
+      <c r="E8" s="2">
+        <v>93.36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2522</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
+      <c r="C14" s="2">
+        <v>1679</v>
+      </c>
+      <c r="D14" s="2">
+        <v>33.549999999999997</v>
+      </c>
+      <c r="E14" s="2">
+        <v>33.549999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Novas otimizações para a consulta 1 - Adição do script para criar as materialized views - Atualização da tabela de tempos
Co-authored-by: Bianca Gomes <bgsrd@outlook.com>
</commit_message>
<xml_diff>
--- a/Fase 03 - SBD (Consultas SQL e Otimização)/Tempos.xlsx
+++ b/Fase 03 - SBD (Consultas SQL e Otimização)/Tempos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\educa_brasil\Fase 03 - SBD (Consultas SQL e Otimização)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pietr\pietrozuntini@gmail.com\Ufscar\Perfil 5\Projeto Integrado (WEB + SBD)\Repositório\Fase 03 - SBD (Consultas SQL e Otimização)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC00FC7-4AB1-48FF-A3DB-51CF45557193}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51310BB-D657-4185-8D52-A6D2D9DD23DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{60C1C061-DBD4-48AD-A7F9-20614BF445A7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Testes</t>
   </si>
@@ -42,9 +42,6 @@
     <t>IN</t>
   </si>
   <si>
-    <t>ÍNDICE</t>
-  </si>
-  <si>
     <t>LIKE</t>
   </si>
   <si>
@@ -64,6 +61,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ÍNDICE (nome_escola)</t>
+  </si>
+  <si>
+    <t>MATERIALIZED VIEW</t>
+  </si>
+  <si>
+    <t>ÍNDICE (co_distrito)</t>
   </si>
 </sst>
 </file>
@@ -122,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -140,6 +146,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0204754B-D6F4-4E2C-9215-C6E014B7E421}">
-  <dimension ref="B2:E16"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B4" sqref="B4:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,27 +488,27 @@
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
         <v>30246</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -515,7 +527,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
         <v>16504</v>
@@ -529,7 +541,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2">
         <v>2008</v>
@@ -541,64 +553,92 @@
         <v>93.36</v>
       </c>
     </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1613</v>
+      </c>
+      <c r="D9" s="8">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="E9" s="8">
+        <v>94.66</v>
+      </c>
+    </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8">
+        <v>482</v>
+      </c>
+      <c r="D10" s="8">
+        <v>70.11</v>
+      </c>
+      <c r="E10" s="8">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="C18" s="2">
+        <v>2522</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2522</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C19" s="2">
         <v>1679</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D19" s="2">
         <v>33.549999999999997</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E19" s="2">
         <v>33.549999999999997</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>